<commit_message>
Creating noun declension table
</commit_message>
<xml_diff>
--- a/TsakonianDB/tables/main.xlsx
+++ b/TsakonianDB/tables/main.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jgcha\Desktop\Python\Códigos\Tsakonian tools\TsakonianDB\tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{420FBAB1-96D4-4611-B928-20446D2F7D3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AD11CF7-7DA0-4AE4-B36B-B1767B9B927A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="670" uniqueCount="478">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="667" uniqueCount="476">
   <si>
     <t>tsakonian</t>
   </si>
@@ -1026,9 +1026,6 @@
     <t>άγο</t>
   </si>
   <si>
-    <t>αλογο</t>
-  </si>
-  <si>
     <t>άσου</t>
   </si>
   <si>
@@ -1261,9 +1258,6 @@
   </si>
   <si>
     <t>αχλάδι</t>
-  </si>
-  <si>
-    <t>Α6</t>
   </si>
   <si>
     <t>άντε</t>
@@ -1501,10 +1495,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1608,10 +1601,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{026E7425-6AE1-4445-B5B5-159D1B7680D9}" name="Tabla1" displayName="Tabla1" ref="A1:D233" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
-  <autoFilter ref="A1:D233" xr:uid="{026E7425-6AE1-4445-B5B5-159D1B7680D9}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D178">
-    <sortCondition ref="A1:A178"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{026E7425-6AE1-4445-B5B5-159D1B7680D9}" name="Tabla1" displayName="Tabla1" ref="A1:D232" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
+  <autoFilter ref="A1:D232" xr:uid="{026E7425-6AE1-4445-B5B5-159D1B7680D9}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D232">
+    <sortCondition ref="A1:A232"/>
   </sortState>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{FA2F0861-8915-4E2E-B6DC-B7DD84954D84}" name="tsakonian" dataDxfId="3"/>
@@ -1886,10 +1879,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D233"/>
+  <dimension ref="A1:D232"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A175" workbookViewId="0">
-      <selection activeCell="D200" sqref="D200"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="21" x14ac:dyDescent="0.35"/>
@@ -1927,13 +1920,13 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
-        <v>332</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>333</v>
+        <v>372</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>373</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>377</v>
+        <v>355</v>
       </c>
       <c r="D3" s="1">
         <v>1</v>
@@ -1941,10 +1934,13 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
-        <v>303</v>
+        <v>332</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>304</v>
+        <v>447</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>352</v>
       </c>
       <c r="D4" s="1">
         <v>1</v>
@@ -1952,13 +1948,10 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
-        <v>354</v>
+        <v>303</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>355</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>356</v>
+        <v>304</v>
       </c>
       <c r="D5" s="1">
         <v>1</v>
@@ -1966,13 +1959,13 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
-        <v>351</v>
+        <v>353</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>352</v>
+        <v>354</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>353</v>
+        <v>355</v>
       </c>
       <c r="D6" s="1">
         <v>1</v>
@@ -1980,13 +1973,13 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
-        <v>167</v>
+        <v>363</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>168</v>
+        <v>364</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>230</v>
+        <v>266</v>
       </c>
       <c r="D7" s="1">
         <v>1</v>
@@ -1994,13 +1987,13 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
-        <v>209</v>
+        <v>433</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>210</v>
+        <v>434</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>230</v>
+        <v>409</v>
       </c>
       <c r="D8" s="1">
         <v>1</v>
@@ -2008,13 +2001,13 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
-        <v>163</v>
+        <v>458</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>164</v>
+        <v>457</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>230</v>
+        <v>355</v>
       </c>
       <c r="D9" s="1">
         <v>1</v>
@@ -2022,10 +2015,13 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
-        <v>297</v>
+        <v>350</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>298</v>
+        <v>351</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>352</v>
       </c>
       <c r="D10" s="1">
         <v>1</v>
@@ -2033,10 +2029,10 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
-        <v>191</v>
+        <v>167</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>192</v>
+        <v>168</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>230</v>
@@ -2047,10 +2043,13 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
-        <v>282</v>
+        <v>209</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>282</v>
+        <v>210</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>230</v>
       </c>
       <c r="D12" s="1">
         <v>1</v>
@@ -2058,13 +2057,13 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
-        <v>175</v>
+        <v>429</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>176</v>
+        <v>430</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>230</v>
+        <v>415</v>
       </c>
       <c r="D13" s="1">
         <v>1</v>
@@ -2072,13 +2071,13 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
-        <v>12</v>
+        <v>163</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>13</v>
+        <v>164</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>324</v>
+        <v>230</v>
       </c>
       <c r="D14" s="1">
         <v>1</v>
@@ -2086,13 +2085,10 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
-        <v>165</v>
+        <v>297</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>166</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>230</v>
+        <v>298</v>
       </c>
       <c r="D15" s="1">
         <v>1</v>
@@ -2100,10 +2096,10 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
-        <v>148</v>
+        <v>191</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>149</v>
+        <v>192</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>230</v>
@@ -2114,13 +2110,10 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
-        <v>96</v>
+        <v>282</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>324</v>
+        <v>282</v>
       </c>
       <c r="D17" s="1">
         <v>1</v>
@@ -2128,13 +2121,13 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
-        <v>173</v>
+        <v>411</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>174</v>
+        <v>412</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>230</v>
+        <v>400</v>
       </c>
       <c r="D18" s="1">
         <v>1</v>
@@ -2142,10 +2135,13 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
-        <v>295</v>
+        <v>175</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>296</v>
+        <v>176</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>230</v>
       </c>
       <c r="D19" s="1">
         <v>1</v>
@@ -2153,13 +2149,13 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
-        <v>93</v>
+        <v>398</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>94</v>
+        <v>399</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>324</v>
+        <v>400</v>
       </c>
       <c r="D20" s="1">
         <v>1</v>
@@ -2167,10 +2163,10 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="s">
-        <v>73</v>
+        <v>12</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>74</v>
+        <v>13</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>324</v>
@@ -2181,10 +2177,13 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A22" s="1" t="s">
-        <v>250</v>
+        <v>165</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>251</v>
+        <v>166</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>230</v>
       </c>
       <c r="D22" s="1">
         <v>1</v>
@@ -2192,13 +2191,13 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A23" s="1" t="s">
-        <v>98</v>
+        <v>390</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>99</v>
+        <v>391</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>324</v>
+        <v>355</v>
       </c>
       <c r="D23" s="1">
         <v>1</v>
@@ -2206,13 +2205,13 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A24" s="1" t="s">
-        <v>100</v>
+        <v>148</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>101</v>
+        <v>149</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>324</v>
+        <v>230</v>
       </c>
       <c r="D24" s="1">
         <v>1</v>
@@ -2220,10 +2219,10 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A25" s="1" t="s">
-        <v>67</v>
+        <v>96</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>68</v>
+        <v>97</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>324</v>
@@ -2234,13 +2233,13 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A26" s="1" t="s">
-        <v>334</v>
+        <v>173</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>335</v>
+        <v>174</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>324</v>
+        <v>230</v>
       </c>
       <c r="D26" s="1">
         <v>1</v>
@@ -2248,13 +2247,10 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A27" s="1" t="s">
-        <v>132</v>
+        <v>295</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="C27" s="1" t="s">
-        <v>326</v>
+        <v>296</v>
       </c>
       <c r="D27" s="1">
         <v>1</v>
@@ -2262,13 +2258,13 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A28" s="1" t="s">
-        <v>336</v>
+        <v>93</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>337</v>
+        <v>94</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>338</v>
+        <v>324</v>
       </c>
       <c r="D28" s="1">
         <v>1</v>
@@ -2276,13 +2272,13 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A29" s="1" t="s">
-        <v>231</v>
+        <v>73</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>232</v>
+        <v>74</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="D29" s="1">
         <v>1</v>
@@ -2290,10 +2286,10 @@
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A30" s="1" t="s">
-        <v>301</v>
+        <v>250</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>302</v>
+        <v>251</v>
       </c>
       <c r="D30" s="1">
         <v>1</v>
@@ -2301,13 +2297,13 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A31" s="1" t="s">
-        <v>237</v>
+        <v>98</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>238</v>
+        <v>99</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>328</v>
+        <v>324</v>
       </c>
       <c r="D31" s="1">
         <v>1</v>
@@ -2315,13 +2311,13 @@
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A32" s="1" t="s">
-        <v>239</v>
+        <v>100</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>240</v>
+        <v>101</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>328</v>
+        <v>324</v>
       </c>
       <c r="D32" s="1">
         <v>1</v>
@@ -2329,10 +2325,10 @@
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A33" s="1" t="s">
-        <v>48</v>
+        <v>67</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>49</v>
+        <v>68</v>
       </c>
       <c r="C33" s="1" t="s">
         <v>324</v>
@@ -2343,13 +2339,13 @@
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A34" s="1" t="s">
-        <v>83</v>
+        <v>413</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>84</v>
+        <v>414</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>324</v>
+        <v>377</v>
       </c>
       <c r="D34" s="1">
         <v>1</v>
@@ -2357,10 +2353,13 @@
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A35" s="1" t="s">
-        <v>289</v>
+        <v>333</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>290</v>
+        <v>334</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>324</v>
       </c>
       <c r="D35" s="1">
         <v>1</v>
@@ -2368,13 +2367,13 @@
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A36" s="1" t="s">
-        <v>46</v>
+        <v>132</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>47</v>
+        <v>133</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>324</v>
+        <v>326</v>
       </c>
       <c r="D36" s="1">
         <v>1</v>
@@ -2382,13 +2381,13 @@
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A37" s="1" t="s">
-        <v>177</v>
+        <v>416</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>178</v>
+        <v>417</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>230</v>
+        <v>376</v>
       </c>
       <c r="D37" s="1">
         <v>1</v>
@@ -2396,13 +2395,13 @@
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A38" s="1" t="s">
-        <v>89</v>
+        <v>365</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>90</v>
+        <v>366</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>324</v>
+        <v>266</v>
       </c>
       <c r="D38" s="1">
         <v>1</v>
@@ -2410,13 +2409,13 @@
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A39" s="1" t="s">
-        <v>91</v>
+        <v>335</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>92</v>
+        <v>336</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>324</v>
+        <v>337</v>
       </c>
       <c r="D39" s="1">
         <v>1</v>
@@ -2424,13 +2423,13 @@
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A40" s="1" t="s">
-        <v>118</v>
+        <v>427</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>119</v>
+        <v>428</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="D40" s="1">
         <v>1</v>
@@ -2438,13 +2437,13 @@
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A41" s="1" t="s">
-        <v>120</v>
+        <v>267</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>121</v>
+        <v>410</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>324</v>
+        <v>475</v>
       </c>
       <c r="D41" s="1">
         <v>1</v>
@@ -2452,10 +2451,13 @@
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A42" s="1" t="s">
-        <v>311</v>
+        <v>231</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>312</v>
+        <v>232</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>326</v>
       </c>
       <c r="D42" s="1">
         <v>1</v>
@@ -2463,13 +2465,10 @@
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A43" s="1" t="s">
-        <v>269</v>
+        <v>301</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>268</v>
-      </c>
-      <c r="C43" s="1" t="s">
-        <v>325</v>
+        <v>302</v>
       </c>
       <c r="D43" s="1">
         <v>1</v>
@@ -2477,13 +2476,13 @@
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A44" s="1" t="s">
-        <v>38</v>
+        <v>237</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>39</v>
+        <v>238</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>324</v>
+        <v>328</v>
       </c>
       <c r="D44" s="1">
         <v>1</v>
@@ -2491,13 +2490,13 @@
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A45" s="1" t="s">
-        <v>18</v>
+        <v>454</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>19</v>
+        <v>455</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>324</v>
+        <v>266</v>
       </c>
       <c r="D45" s="1">
         <v>1</v>
@@ -2505,13 +2504,13 @@
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A46" s="1" t="s">
-        <v>211</v>
+        <v>239</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>212</v>
+        <v>240</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>230</v>
+        <v>328</v>
       </c>
       <c r="D46" s="1">
         <v>1</v>
@@ -2519,10 +2518,13 @@
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A47" s="1" t="s">
-        <v>254</v>
+        <v>405</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>255</v>
+        <v>406</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>400</v>
       </c>
       <c r="D47" s="1">
         <v>1</v>
@@ -2530,10 +2532,10 @@
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A48" s="1" t="s">
-        <v>127</v>
+        <v>48</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>128</v>
+        <v>49</v>
       </c>
       <c r="C48" s="1" t="s">
         <v>324</v>
@@ -2544,13 +2546,13 @@
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A49" s="1" t="s">
-        <v>215</v>
+        <v>443</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>216</v>
+        <v>444</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>230</v>
+        <v>266</v>
       </c>
       <c r="D49" s="1">
         <v>1</v>
@@ -2558,10 +2560,10 @@
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A50" s="1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C50" s="1" t="s">
         <v>324</v>
@@ -2572,13 +2574,13 @@
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A51" s="1" t="s">
-        <v>87</v>
+        <v>425</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>88</v>
+        <v>426</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>324</v>
+        <v>376</v>
       </c>
       <c r="D51" s="1">
         <v>1</v>
@@ -2586,13 +2588,10 @@
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A52" s="1" t="s">
-        <v>154</v>
+        <v>289</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="C52" s="1" t="s">
-        <v>230</v>
+        <v>290</v>
       </c>
       <c r="D52" s="1">
         <v>1</v>
@@ -2600,10 +2599,10 @@
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A53" s="1" t="s">
-        <v>258</v>
+        <v>46</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>259</v>
+        <v>47</v>
       </c>
       <c r="C53" s="1" t="s">
         <v>324</v>
@@ -2614,13 +2613,13 @@
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A54" s="1" t="s">
-        <v>4</v>
+        <v>456</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>5</v>
+        <v>457</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>324</v>
+        <v>355</v>
       </c>
       <c r="D54" s="1">
         <v>1</v>
@@ -2628,13 +2627,13 @@
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A55" s="1" t="s">
-        <v>79</v>
+        <v>431</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>80</v>
+        <v>432</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>324</v>
+        <v>376</v>
       </c>
       <c r="D55" s="1">
         <v>1</v>
@@ -2642,13 +2641,13 @@
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A56" s="1" t="s">
-        <v>77</v>
+        <v>177</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>78</v>
+        <v>178</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>324</v>
+        <v>230</v>
       </c>
       <c r="D56" s="1">
         <v>1</v>
@@ -2656,13 +2655,13 @@
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A57" s="1" t="s">
-        <v>179</v>
+        <v>89</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>180</v>
+        <v>90</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>230</v>
+        <v>324</v>
       </c>
       <c r="D57" s="1">
         <v>1</v>
@@ -2670,13 +2669,13 @@
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A58" s="1" t="s">
-        <v>243</v>
+        <v>91</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>244</v>
+        <v>92</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="D58" s="1">
         <v>1</v>
@@ -2684,10 +2683,13 @@
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A59" s="1" t="s">
-        <v>285</v>
+        <v>118</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>286</v>
+        <v>119</v>
+      </c>
+      <c r="C59" s="1" t="s">
+        <v>324</v>
       </c>
       <c r="D59" s="1">
         <v>1</v>
@@ -2695,10 +2697,10 @@
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A60" s="1" t="s">
-        <v>54</v>
+        <v>120</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>55</v>
+        <v>121</v>
       </c>
       <c r="C60" s="1" t="s">
         <v>324</v>
@@ -2709,13 +2711,13 @@
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A61" s="1" t="s">
-        <v>56</v>
+        <v>367</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>57</v>
+        <v>368</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>324</v>
+        <v>355</v>
       </c>
       <c r="D61" s="1">
         <v>1</v>
@@ -2723,13 +2725,10 @@
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A62" s="1" t="s">
-        <v>208</v>
+        <v>311</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>203</v>
-      </c>
-      <c r="C62" s="1" t="s">
-        <v>230</v>
+        <v>312</v>
       </c>
       <c r="D62" s="1">
         <v>1</v>
@@ -2737,13 +2736,13 @@
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A63" s="1" t="s">
-        <v>108</v>
+        <v>269</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>109</v>
+        <v>268</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="D63" s="1">
         <v>1</v>
@@ -2751,10 +2750,10 @@
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A64" s="1" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="C64" s="1" t="s">
         <v>324</v>
@@ -2765,13 +2764,13 @@
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A65" s="1" t="s">
-        <v>181</v>
+        <v>18</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>182</v>
+        <v>19</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>230</v>
+        <v>324</v>
       </c>
       <c r="D65" s="1">
         <v>1</v>
@@ -2779,10 +2778,10 @@
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A66" s="1" t="s">
-        <v>183</v>
+        <v>211</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>184</v>
+        <v>212</v>
       </c>
       <c r="C66" s="1" t="s">
         <v>230</v>
@@ -2793,13 +2792,13 @@
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A67" s="1" t="s">
-        <v>114</v>
+        <v>378</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>115</v>
+        <v>379</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>324</v>
+        <v>230</v>
       </c>
       <c r="D67" s="1">
         <v>1</v>
@@ -2807,13 +2806,13 @@
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A68" s="1" t="s">
-        <v>116</v>
+        <v>382</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>117</v>
+        <v>383</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>324</v>
+        <v>230</v>
       </c>
       <c r="D68" s="1">
         <v>1</v>
@@ -2821,13 +2820,13 @@
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A69" s="1" t="s">
-        <v>42</v>
+        <v>401</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>43</v>
+        <v>402</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>324</v>
+        <v>355</v>
       </c>
       <c r="D69" s="1">
         <v>1</v>
@@ -2835,13 +2834,10 @@
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A70" s="1" t="s">
-        <v>58</v>
+        <v>254</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="C70" s="1" t="s">
-        <v>324</v>
+        <v>255</v>
       </c>
       <c r="D70" s="1">
         <v>1</v>
@@ -2849,10 +2845,10 @@
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A71" s="1" t="s">
-        <v>185</v>
+        <v>384</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>186</v>
+        <v>385</v>
       </c>
       <c r="C71" s="1" t="s">
         <v>230</v>
@@ -2863,13 +2859,13 @@
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A72" s="1" t="s">
-        <v>106</v>
+        <v>381</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>107</v>
+        <v>380</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>324</v>
+        <v>230</v>
       </c>
       <c r="D72" s="1">
         <v>1</v>
@@ -2877,13 +2873,13 @@
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A73" s="1" t="s">
-        <v>247</v>
+        <v>127</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>248</v>
+        <v>128</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>249</v>
+        <v>324</v>
       </c>
       <c r="D73" s="1">
         <v>1</v>
@@ -2891,13 +2887,13 @@
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A74" s="1" t="s">
-        <v>247</v>
+        <v>215</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>248</v>
+        <v>216</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>266</v>
+        <v>230</v>
       </c>
       <c r="D74" s="1">
         <v>1</v>
@@ -2905,10 +2901,10 @@
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A75" s="1" t="s">
-        <v>95</v>
+        <v>85</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>9</v>
+        <v>86</v>
       </c>
       <c r="C75" s="1" t="s">
         <v>324</v>
@@ -2919,10 +2915,10 @@
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A76" s="1" t="s">
-        <v>8</v>
+        <v>87</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>9</v>
+        <v>88</v>
       </c>
       <c r="C76" s="1" t="s">
         <v>324</v>
@@ -2933,13 +2929,13 @@
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A77" s="1" t="s">
-        <v>313</v>
+        <v>459</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>314</v>
+        <v>460</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>377</v>
+        <v>266</v>
       </c>
       <c r="D77" s="1">
         <v>1</v>
@@ -2947,13 +2943,13 @@
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A78" s="1" t="s">
-        <v>343</v>
+        <v>154</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>345</v>
+        <v>155</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>346</v>
+        <v>230</v>
       </c>
       <c r="D78" s="1">
         <v>1</v>
@@ -2961,10 +2957,13 @@
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A79" s="1" t="s">
-        <v>293</v>
+        <v>258</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>294</v>
+        <v>259</v>
+      </c>
+      <c r="C79" s="1" t="s">
+        <v>324</v>
       </c>
       <c r="D79" s="1">
         <v>1</v>
@@ -2972,13 +2971,13 @@
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A80" s="1" t="s">
-        <v>339</v>
+        <v>4</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>340</v>
+        <v>5</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>341</v>
+        <v>324</v>
       </c>
       <c r="D80" s="1">
         <v>1</v>
@@ -2986,13 +2985,13 @@
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A81" s="1" t="s">
-        <v>131</v>
+        <v>396</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>131</v>
+        <v>397</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>230</v>
+        <v>355</v>
       </c>
       <c r="D81" s="1">
         <v>1</v>
@@ -3000,13 +2999,13 @@
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A82" s="1" t="s">
-        <v>156</v>
+        <v>79</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>157</v>
+        <v>80</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>230</v>
+        <v>324</v>
       </c>
       <c r="D82" s="1">
         <v>1</v>
@@ -3014,10 +3013,13 @@
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A83" s="1" t="s">
-        <v>260</v>
+        <v>77</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>261</v>
+        <v>78</v>
+      </c>
+      <c r="C83" s="1" t="s">
+        <v>324</v>
       </c>
       <c r="D83" s="1">
         <v>1</v>
@@ -3025,10 +3027,13 @@
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A84" s="1" t="s">
-        <v>252</v>
+        <v>179</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>253</v>
+        <v>180</v>
+      </c>
+      <c r="C84" s="1" t="s">
+        <v>230</v>
       </c>
       <c r="D84" s="1">
         <v>1</v>
@@ -3036,13 +3041,13 @@
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A85" s="1" t="s">
-        <v>235</v>
+        <v>243</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>236</v>
+        <v>244</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="D85" s="1">
         <v>1</v>
@@ -3050,13 +3055,10 @@
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A86" s="1" t="s">
-        <v>75</v>
+        <v>285</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="C86" s="1" t="s">
-        <v>324</v>
+        <v>286</v>
       </c>
       <c r="D86" s="1">
         <v>1</v>
@@ -3064,10 +3066,10 @@
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A87" s="1" t="s">
-        <v>30</v>
+        <v>54</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>31</v>
+        <v>55</v>
       </c>
       <c r="C87" s="1" t="s">
         <v>324</v>
@@ -3078,10 +3080,10 @@
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A88" s="1" t="s">
-        <v>34</v>
+        <v>56</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>35</v>
+        <v>57</v>
       </c>
       <c r="C88" s="1" t="s">
         <v>324</v>
@@ -3092,13 +3094,13 @@
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A89" s="1" t="s">
-        <v>32</v>
+        <v>208</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>33</v>
+        <v>203</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>324</v>
+        <v>230</v>
       </c>
       <c r="D89" s="1">
         <v>1</v>
@@ -3106,13 +3108,13 @@
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A90" s="1" t="s">
-        <v>81</v>
+        <v>439</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>82</v>
+        <v>440</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>324</v>
+        <v>371</v>
       </c>
       <c r="D90" s="1">
         <v>1</v>
@@ -3120,10 +3122,10 @@
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A91" s="1" t="s">
-        <v>124</v>
+        <v>108</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>125</v>
+        <v>109</v>
       </c>
       <c r="C91" s="1" t="s">
         <v>324</v>
@@ -3134,10 +3136,10 @@
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A92" s="1" t="s">
-        <v>124</v>
+        <v>44</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>126</v>
+        <v>45</v>
       </c>
       <c r="C92" s="1" t="s">
         <v>324</v>
@@ -3148,13 +3150,13 @@
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A93" s="1" t="s">
-        <v>69</v>
+        <v>181</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>70</v>
+        <v>182</v>
       </c>
       <c r="C93" s="1" t="s">
-        <v>324</v>
+        <v>230</v>
       </c>
       <c r="D93" s="1">
         <v>1</v>
@@ -3162,10 +3164,10 @@
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A94" s="1" t="s">
-        <v>217</v>
+        <v>183</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>218</v>
+        <v>184</v>
       </c>
       <c r="C94" s="1" t="s">
         <v>230</v>
@@ -3176,10 +3178,10 @@
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A95" s="1" t="s">
-        <v>61</v>
+        <v>114</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>62</v>
+        <v>115</v>
       </c>
       <c r="C95" s="1" t="s">
         <v>324</v>
@@ -3190,10 +3192,10 @@
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A96" s="1" t="s">
-        <v>24</v>
+        <v>116</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>25</v>
+        <v>117</v>
       </c>
       <c r="C96" s="1" t="s">
         <v>324</v>
@@ -3204,10 +3206,10 @@
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A97" s="1" t="s">
-        <v>22</v>
+        <v>42</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>23</v>
+        <v>43</v>
       </c>
       <c r="C97" s="1" t="s">
         <v>324</v>
@@ -3218,10 +3220,13 @@
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A98" s="1" t="s">
-        <v>309</v>
+        <v>58</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>310</v>
+        <v>57</v>
+      </c>
+      <c r="C98" s="1" t="s">
+        <v>324</v>
       </c>
       <c r="D98" s="1">
         <v>1</v>
@@ -3229,10 +3234,10 @@
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A99" s="1" t="s">
-        <v>219</v>
+        <v>185</v>
       </c>
       <c r="B99" s="1" t="s">
-        <v>220</v>
+        <v>186</v>
       </c>
       <c r="C99" s="1" t="s">
         <v>230</v>
@@ -3243,10 +3248,10 @@
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A100" s="1" t="s">
-        <v>36</v>
+        <v>106</v>
       </c>
       <c r="B100" s="1" t="s">
-        <v>37</v>
+        <v>107</v>
       </c>
       <c r="C100" s="1" t="s">
         <v>324</v>
@@ -3257,13 +3262,13 @@
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A101" s="1" t="s">
-        <v>245</v>
+        <v>247</v>
       </c>
       <c r="B101" s="1" t="s">
-        <v>246</v>
+        <v>248</v>
       </c>
       <c r="C101" s="1" t="s">
-        <v>329</v>
+        <v>249</v>
       </c>
       <c r="D101" s="1">
         <v>1</v>
@@ -3271,13 +3276,13 @@
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A102" s="1" t="s">
-        <v>224</v>
+        <v>247</v>
       </c>
       <c r="B102" s="1" t="s">
-        <v>225</v>
+        <v>248</v>
       </c>
       <c r="C102" s="1" t="s">
-        <v>230</v>
+        <v>266</v>
       </c>
       <c r="D102" s="1">
         <v>1</v>
@@ -3285,10 +3290,13 @@
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A103" s="1" t="s">
-        <v>262</v>
+        <v>469</v>
       </c>
       <c r="B103" s="1" t="s">
-        <v>262</v>
+        <v>470</v>
+      </c>
+      <c r="C103" s="1" t="s">
+        <v>358</v>
       </c>
       <c r="D103" s="1">
         <v>1</v>
@@ -3296,13 +3304,13 @@
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A104" s="1" t="s">
-        <v>193</v>
+        <v>95</v>
       </c>
       <c r="B104" s="1" t="s">
-        <v>194</v>
+        <v>9</v>
       </c>
       <c r="C104" s="1" t="s">
-        <v>230</v>
+        <v>324</v>
       </c>
       <c r="D104" s="1">
         <v>1</v>
@@ -3310,13 +3318,13 @@
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A105" s="1" t="s">
-        <v>197</v>
+        <v>8</v>
       </c>
       <c r="B105" s="1" t="s">
-        <v>198</v>
+        <v>9</v>
       </c>
       <c r="C105" s="1" t="s">
-        <v>230</v>
+        <v>324</v>
       </c>
       <c r="D105" s="1">
         <v>1</v>
@@ -3324,10 +3332,13 @@
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A106" s="1" t="s">
-        <v>307</v>
+        <v>441</v>
       </c>
       <c r="B106" s="1" t="s">
-        <v>308</v>
+        <v>442</v>
+      </c>
+      <c r="C106" s="1" t="s">
+        <v>355</v>
       </c>
       <c r="D106" s="1">
         <v>1</v>
@@ -3335,13 +3346,13 @@
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A107" s="1" t="s">
-        <v>187</v>
+        <v>394</v>
       </c>
       <c r="B107" s="1" t="s">
-        <v>188</v>
+        <v>395</v>
       </c>
       <c r="C107" s="1" t="s">
-        <v>230</v>
+        <v>355</v>
       </c>
       <c r="D107" s="1">
         <v>1</v>
@@ -3349,13 +3360,13 @@
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A108" s="1" t="s">
-        <v>195</v>
+        <v>437</v>
       </c>
       <c r="B108" s="1" t="s">
-        <v>196</v>
+        <v>438</v>
       </c>
       <c r="C108" s="1" t="s">
-        <v>230</v>
+        <v>352</v>
       </c>
       <c r="D108" s="1">
         <v>1</v>
@@ -3363,13 +3374,13 @@
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A109" s="1" t="s">
-        <v>14</v>
+        <v>313</v>
       </c>
       <c r="B109" s="1" t="s">
-        <v>15</v>
+        <v>314</v>
       </c>
       <c r="C109" s="1" t="s">
-        <v>324</v>
+        <v>376</v>
       </c>
       <c r="D109" s="1">
         <v>1</v>
@@ -3377,13 +3388,13 @@
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A110" s="1" t="s">
-        <v>16</v>
+        <v>451</v>
       </c>
       <c r="B110" s="1" t="s">
-        <v>17</v>
+        <v>449</v>
       </c>
       <c r="C110" s="1" t="s">
-        <v>324</v>
+        <v>355</v>
       </c>
       <c r="D110" s="1">
         <v>1</v>
@@ -3391,13 +3402,13 @@
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A111" s="1" t="s">
-        <v>199</v>
+        <v>386</v>
       </c>
       <c r="B111" s="1" t="s">
-        <v>188</v>
+        <v>387</v>
       </c>
       <c r="C111" s="1" t="s">
-        <v>230</v>
+        <v>415</v>
       </c>
       <c r="D111" s="1">
         <v>1</v>
@@ -3405,13 +3416,13 @@
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A112" s="1" t="s">
-        <v>221</v>
+        <v>422</v>
       </c>
       <c r="B112" s="1" t="s">
-        <v>222</v>
+        <v>423</v>
       </c>
       <c r="C112" s="1" t="s">
-        <v>230</v>
+        <v>424</v>
       </c>
       <c r="D112" s="1">
         <v>1</v>
@@ -3419,13 +3430,13 @@
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A113" s="1" t="s">
-        <v>342</v>
+        <v>463</v>
       </c>
       <c r="B113" s="1" t="s">
-        <v>344</v>
+        <v>464</v>
       </c>
       <c r="C113" s="1" t="s">
-        <v>338</v>
+        <v>266</v>
       </c>
       <c r="D113" s="1">
         <v>1</v>
@@ -3433,10 +3444,13 @@
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A114" s="1" t="s">
-        <v>276</v>
+        <v>407</v>
       </c>
       <c r="B114" s="1" t="s">
-        <v>277</v>
+        <v>408</v>
+      </c>
+      <c r="C114" s="1" t="s">
+        <v>409</v>
       </c>
       <c r="D114" s="1">
         <v>1</v>
@@ -3444,13 +3458,13 @@
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A115" s="1" t="s">
-        <v>206</v>
+        <v>342</v>
       </c>
       <c r="B115" s="1" t="s">
-        <v>207</v>
+        <v>344</v>
       </c>
       <c r="C115" s="1" t="s">
-        <v>230</v>
+        <v>345</v>
       </c>
       <c r="D115" s="1">
         <v>1</v>
@@ -3458,13 +3472,10 @@
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A116" s="1" t="s">
-        <v>10</v>
+        <v>293</v>
       </c>
       <c r="B116" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C116" s="1" t="s">
-        <v>324</v>
+        <v>294</v>
       </c>
       <c r="D116" s="1">
         <v>1</v>
@@ -3472,13 +3483,13 @@
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A117" s="1" t="s">
-        <v>160</v>
+        <v>338</v>
       </c>
       <c r="B117" s="1" t="s">
-        <v>161</v>
+        <v>339</v>
       </c>
       <c r="C117" s="1" t="s">
-        <v>230</v>
+        <v>340</v>
       </c>
       <c r="D117" s="1">
         <v>1</v>
@@ -3486,10 +3497,10 @@
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A118" s="1" t="s">
-        <v>200</v>
+        <v>131</v>
       </c>
       <c r="B118" s="1" t="s">
-        <v>201</v>
+        <v>131</v>
       </c>
       <c r="C118" s="1" t="s">
         <v>230</v>
@@ -3500,13 +3511,13 @@
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A119" s="1" t="s">
-        <v>122</v>
+        <v>156</v>
       </c>
       <c r="B119" s="1" t="s">
-        <v>123</v>
+        <v>157</v>
       </c>
       <c r="C119" s="1" t="s">
-        <v>324</v>
+        <v>230</v>
       </c>
       <c r="D119" s="1">
         <v>1</v>
@@ -3514,10 +3525,13 @@
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A120" s="1" t="s">
-        <v>274</v>
+        <v>473</v>
       </c>
       <c r="B120" s="1" t="s">
-        <v>273</v>
+        <v>474</v>
+      </c>
+      <c r="C120" s="1" t="s">
+        <v>475</v>
       </c>
       <c r="D120" s="1">
         <v>1</v>
@@ -3525,13 +3539,10 @@
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A121" s="1" t="s">
-        <v>223</v>
+        <v>260</v>
       </c>
       <c r="B121" s="1" t="s">
-        <v>184</v>
-      </c>
-      <c r="C121" s="1" t="s">
-        <v>230</v>
+        <v>261</v>
       </c>
       <c r="D121" s="1">
         <v>1</v>
@@ -3539,13 +3550,10 @@
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A122" s="1" t="s">
-        <v>142</v>
+        <v>252</v>
       </c>
       <c r="B122" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="C122" s="1" t="s">
-        <v>230</v>
+        <v>253</v>
       </c>
       <c r="D122" s="1">
         <v>1</v>
@@ -3553,10 +3561,13 @@
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A123" s="1" t="s">
-        <v>256</v>
+        <v>235</v>
       </c>
       <c r="B123" s="1" t="s">
-        <v>257</v>
+        <v>236</v>
+      </c>
+      <c r="C123" s="1" t="s">
+        <v>327</v>
       </c>
       <c r="D123" s="1">
         <v>1</v>
@@ -3564,10 +3575,10 @@
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A124" s="1" t="s">
-        <v>20</v>
+        <v>75</v>
       </c>
       <c r="B124" s="1" t="s">
-        <v>21</v>
+        <v>76</v>
       </c>
       <c r="C124" s="1" t="s">
         <v>324</v>
@@ -3578,13 +3589,13 @@
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A125" s="1" t="s">
-        <v>315</v>
+        <v>448</v>
       </c>
       <c r="B125" s="1" t="s">
-        <v>316</v>
+        <v>450</v>
       </c>
       <c r="C125" s="1" t="s">
-        <v>317</v>
+        <v>266</v>
       </c>
       <c r="D125" s="1">
         <v>1</v>
@@ -3592,13 +3603,13 @@
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A126" s="1" t="s">
-        <v>189</v>
+        <v>471</v>
       </c>
       <c r="B126" s="1" t="s">
-        <v>190</v>
+        <v>472</v>
       </c>
       <c r="C126" s="1" t="s">
-        <v>230</v>
+        <v>355</v>
       </c>
       <c r="D126" s="1">
         <v>1</v>
@@ -3606,13 +3617,13 @@
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A127" s="1" t="s">
-        <v>162</v>
+        <v>30</v>
       </c>
       <c r="B127" s="1" t="s">
-        <v>161</v>
+        <v>31</v>
       </c>
       <c r="C127" s="1" t="s">
-        <v>230</v>
+        <v>324</v>
       </c>
       <c r="D127" s="1">
         <v>1</v>
@@ -3620,13 +3631,13 @@
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A128" s="1" t="s">
-        <v>241</v>
+        <v>34</v>
       </c>
       <c r="B128" s="1" t="s">
-        <v>242</v>
+        <v>35</v>
       </c>
       <c r="C128" s="1" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="D128" s="1">
         <v>1</v>
@@ -3634,10 +3645,10 @@
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A129" s="1" t="s">
-        <v>71</v>
+        <v>32</v>
       </c>
       <c r="B129" s="1" t="s">
-        <v>72</v>
+        <v>33</v>
       </c>
       <c r="C129" s="1" t="s">
         <v>324</v>
@@ -3648,13 +3659,13 @@
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A130" s="1" t="s">
-        <v>144</v>
+        <v>81</v>
       </c>
       <c r="B130" s="1" t="s">
-        <v>145</v>
+        <v>82</v>
       </c>
       <c r="C130" s="1" t="s">
-        <v>230</v>
+        <v>324</v>
       </c>
       <c r="D130" s="1">
         <v>1</v>
@@ -3662,13 +3673,13 @@
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A131" s="1" t="s">
-        <v>213</v>
+        <v>124</v>
       </c>
       <c r="B131" s="1" t="s">
-        <v>214</v>
+        <v>125</v>
       </c>
       <c r="C131" s="1" t="s">
-        <v>230</v>
+        <v>324</v>
       </c>
       <c r="D131" s="1">
         <v>1</v>
@@ -3676,10 +3687,13 @@
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A132" s="1" t="s">
-        <v>278</v>
+        <v>124</v>
       </c>
       <c r="B132" s="1" t="s">
-        <v>279</v>
+        <v>126</v>
+      </c>
+      <c r="C132" s="1" t="s">
+        <v>324</v>
       </c>
       <c r="D132" s="1">
         <v>1</v>
@@ -3687,13 +3701,13 @@
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A133" s="1" t="s">
-        <v>349</v>
+        <v>69</v>
       </c>
       <c r="B133" s="1" t="s">
-        <v>350</v>
+        <v>70</v>
       </c>
       <c r="C133" s="1" t="s">
-        <v>341</v>
+        <v>324</v>
       </c>
       <c r="D133" s="1">
         <v>1</v>
@@ -3701,10 +3715,10 @@
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A134" s="1" t="s">
-        <v>226</v>
+        <v>217</v>
       </c>
       <c r="B134" s="1" t="s">
-        <v>227</v>
+        <v>218</v>
       </c>
       <c r="C134" s="1" t="s">
         <v>230</v>
@@ -3715,13 +3729,13 @@
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A135" s="1" t="s">
-        <v>6</v>
+        <v>61</v>
       </c>
       <c r="B135" s="1" t="s">
-        <v>7</v>
+        <v>62</v>
       </c>
       <c r="C135" s="1" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="D135" s="1">
         <v>1</v>
@@ -3729,10 +3743,13 @@
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A136" s="1" t="s">
-        <v>299</v>
+        <v>435</v>
       </c>
       <c r="B136" s="1" t="s">
-        <v>300</v>
+        <v>436</v>
+      </c>
+      <c r="C136" s="1" t="s">
+        <v>409</v>
       </c>
       <c r="D136" s="1">
         <v>1</v>
@@ -3740,10 +3757,13 @@
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A137" s="1" t="s">
-        <v>305</v>
+        <v>24</v>
       </c>
       <c r="B137" s="1" t="s">
-        <v>306</v>
+        <v>25</v>
+      </c>
+      <c r="C137" s="1" t="s">
+        <v>324</v>
       </c>
       <c r="D137" s="1">
         <v>1</v>
@@ -3751,10 +3771,10 @@
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A138" s="1" t="s">
-        <v>102</v>
+        <v>22</v>
       </c>
       <c r="B138" s="1" t="s">
-        <v>103</v>
+        <v>23</v>
       </c>
       <c r="C138" s="1" t="s">
         <v>324</v>
@@ -3765,13 +3785,10 @@
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A139" s="1" t="s">
-        <v>104</v>
+        <v>309</v>
       </c>
       <c r="B139" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="C139" s="1" t="s">
-        <v>324</v>
+        <v>310</v>
       </c>
       <c r="D139" s="1">
         <v>1</v>
@@ -3779,10 +3796,10 @@
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A140" s="1" t="s">
-        <v>228</v>
+        <v>219</v>
       </c>
       <c r="B140" s="1" t="s">
-        <v>229</v>
+        <v>220</v>
       </c>
       <c r="C140" s="1" t="s">
         <v>230</v>
@@ -3793,10 +3810,10 @@
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A141" s="1" t="s">
-        <v>52</v>
+        <v>36</v>
       </c>
       <c r="B141" s="1" t="s">
-        <v>53</v>
+        <v>37</v>
       </c>
       <c r="C141" s="1" t="s">
         <v>324</v>
@@ -3807,13 +3824,13 @@
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A142" s="1" t="s">
-        <v>50</v>
+        <v>245</v>
       </c>
       <c r="B142" s="1" t="s">
-        <v>51</v>
+        <v>246</v>
       </c>
       <c r="C142" s="1" t="s">
-        <v>324</v>
+        <v>329</v>
       </c>
       <c r="D142" s="1">
         <v>1</v>
@@ -3821,13 +3838,13 @@
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A143" s="1" t="s">
-        <v>150</v>
+        <v>392</v>
       </c>
       <c r="B143" s="1" t="s">
-        <v>151</v>
+        <v>393</v>
       </c>
       <c r="C143" s="1" t="s">
-        <v>230</v>
+        <v>355</v>
       </c>
       <c r="D143" s="1">
         <v>1</v>
@@ -3835,10 +3852,10 @@
     </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A144" s="1" t="s">
-        <v>204</v>
+        <v>224</v>
       </c>
       <c r="B144" s="1" t="s">
-        <v>205</v>
+        <v>225</v>
       </c>
       <c r="C144" s="1" t="s">
         <v>230</v>
@@ -3849,13 +3866,10 @@
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A145" s="1" t="s">
-        <v>169</v>
+        <v>262</v>
       </c>
       <c r="B145" s="1" t="s">
-        <v>170</v>
-      </c>
-      <c r="C145" s="1" t="s">
-        <v>230</v>
+        <v>262</v>
       </c>
       <c r="D145" s="1">
         <v>1</v>
@@ -3863,10 +3877,10 @@
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A146" s="1" t="s">
-        <v>152</v>
+        <v>193</v>
       </c>
       <c r="B146" s="1" t="s">
-        <v>153</v>
+        <v>194</v>
       </c>
       <c r="C146" s="1" t="s">
         <v>230</v>
@@ -3877,10 +3891,10 @@
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A147" s="1" t="s">
-        <v>171</v>
+        <v>197</v>
       </c>
       <c r="B147" s="1" t="s">
-        <v>172</v>
+        <v>198</v>
       </c>
       <c r="C147" s="1" t="s">
         <v>230</v>
@@ -3891,13 +3905,10 @@
     </row>
     <row r="148" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A148" s="1" t="s">
-        <v>134</v>
+        <v>307</v>
       </c>
       <c r="B148" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="C148" s="1" t="s">
-        <v>230</v>
+        <v>308</v>
       </c>
       <c r="D148" s="1">
         <v>1</v>
@@ -3905,10 +3916,13 @@
     </row>
     <row r="149" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A149" s="1" t="s">
-        <v>272</v>
+        <v>445</v>
       </c>
       <c r="B149" s="1" t="s">
-        <v>275</v>
+        <v>446</v>
+      </c>
+      <c r="C149" s="1" t="s">
+        <v>400</v>
       </c>
       <c r="D149" s="1">
         <v>1</v>
@@ -3916,10 +3930,13 @@
     </row>
     <row r="150" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A150" s="1" t="s">
-        <v>265</v>
+        <v>187</v>
       </c>
       <c r="B150" s="1" t="s">
-        <v>265</v>
+        <v>188</v>
+      </c>
+      <c r="C150" s="1" t="s">
+        <v>230</v>
       </c>
       <c r="D150" s="1">
         <v>1</v>
@@ -3927,10 +3944,10 @@
     </row>
     <row r="151" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A151" s="1" t="s">
-        <v>136</v>
+        <v>195</v>
       </c>
       <c r="B151" s="1" t="s">
-        <v>137</v>
+        <v>196</v>
       </c>
       <c r="C151" s="1" t="s">
         <v>230</v>
@@ -3941,13 +3958,13 @@
     </row>
     <row r="152" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A152" s="1" t="s">
-        <v>138</v>
+        <v>14</v>
       </c>
       <c r="B152" s="1" t="s">
-        <v>139</v>
+        <v>15</v>
       </c>
       <c r="C152" s="1" t="s">
-        <v>230</v>
+        <v>324</v>
       </c>
       <c r="D152" s="1">
         <v>1</v>
@@ -3955,13 +3972,13 @@
     </row>
     <row r="153" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A153" s="1" t="s">
-        <v>140</v>
+        <v>16</v>
       </c>
       <c r="B153" s="1" t="s">
-        <v>141</v>
+        <v>17</v>
       </c>
       <c r="C153" s="1" t="s">
-        <v>230</v>
+        <v>324</v>
       </c>
       <c r="D153" s="1">
         <v>1</v>
@@ -3969,10 +3986,10 @@
     </row>
     <row r="154" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A154" s="1" t="s">
-        <v>129</v>
+        <v>199</v>
       </c>
       <c r="B154" s="1" t="s">
-        <v>130</v>
+        <v>188</v>
       </c>
       <c r="C154" s="1" t="s">
         <v>230</v>
@@ -3983,13 +4000,13 @@
     </row>
     <row r="155" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A155" s="1" t="s">
-        <v>318</v>
+        <v>221</v>
       </c>
       <c r="B155" s="1" t="s">
-        <v>319</v>
+        <v>222</v>
       </c>
       <c r="C155" s="1" t="s">
-        <v>249</v>
+        <v>230</v>
       </c>
       <c r="D155" s="1">
         <v>1</v>
@@ -3997,13 +4014,13 @@
     </row>
     <row r="156" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A156" s="1" t="s">
-        <v>59</v>
+        <v>467</v>
       </c>
       <c r="B156" s="1" t="s">
-        <v>60</v>
+        <v>468</v>
       </c>
       <c r="C156" s="1" t="s">
-        <v>324</v>
+        <v>352</v>
       </c>
       <c r="D156" s="1">
         <v>1</v>
@@ -4011,13 +4028,13 @@
     </row>
     <row r="157" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A157" s="1" t="s">
-        <v>320</v>
+        <v>341</v>
       </c>
       <c r="B157" s="1" t="s">
-        <v>321</v>
+        <v>343</v>
       </c>
       <c r="C157" s="1" t="s">
-        <v>360</v>
+        <v>337</v>
       </c>
       <c r="D157" s="1">
         <v>1</v>
@@ -4025,13 +4042,10 @@
     </row>
     <row r="158" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A158" s="1" t="s">
-        <v>357</v>
+        <v>276</v>
       </c>
       <c r="B158" s="1" t="s">
-        <v>358</v>
-      </c>
-      <c r="C158" s="1" t="s">
-        <v>359</v>
+        <v>277</v>
       </c>
       <c r="D158" s="1">
         <v>1</v>
@@ -4039,10 +4053,10 @@
     </row>
     <row r="159" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A159" s="1" t="s">
-        <v>158</v>
+        <v>206</v>
       </c>
       <c r="B159" s="1" t="s">
-        <v>159</v>
+        <v>207</v>
       </c>
       <c r="C159" s="1" t="s">
         <v>230</v>
@@ -4053,10 +4067,13 @@
     </row>
     <row r="160" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A160" s="1" t="s">
-        <v>270</v>
+        <v>10</v>
       </c>
       <c r="B160" s="1" t="s">
-        <v>271</v>
+        <v>11</v>
+      </c>
+      <c r="C160" s="1" t="s">
+        <v>324</v>
       </c>
       <c r="D160" s="1">
         <v>1</v>
@@ -4064,13 +4081,13 @@
     </row>
     <row r="161" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A161" s="1" t="s">
-        <v>322</v>
+        <v>160</v>
       </c>
       <c r="B161" s="1" t="s">
-        <v>323</v>
+        <v>161</v>
       </c>
       <c r="C161" s="1" t="s">
-        <v>324</v>
+        <v>230</v>
       </c>
       <c r="D161" s="1">
         <v>1</v>
@@ -4078,10 +4095,10 @@
     </row>
     <row r="162" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A162" s="1" t="s">
-        <v>146</v>
+        <v>200</v>
       </c>
       <c r="B162" s="1" t="s">
-        <v>147</v>
+        <v>201</v>
       </c>
       <c r="C162" s="1" t="s">
         <v>230</v>
@@ -4092,10 +4109,10 @@
     </row>
     <row r="163" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A163" s="1" t="s">
-        <v>40</v>
+        <v>122</v>
       </c>
       <c r="B163" s="1" t="s">
-        <v>41</v>
+        <v>123</v>
       </c>
       <c r="C163" s="1" t="s">
         <v>324</v>
@@ -4106,10 +4123,10 @@
     </row>
     <row r="164" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A164" s="1" t="s">
-        <v>280</v>
+        <v>274</v>
       </c>
       <c r="B164" s="1" t="s">
-        <v>281</v>
+        <v>273</v>
       </c>
       <c r="D164" s="1">
         <v>1</v>
@@ -4117,13 +4134,13 @@
     </row>
     <row r="165" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A165" s="1" t="s">
-        <v>347</v>
+        <v>223</v>
       </c>
       <c r="B165" s="1" t="s">
-        <v>348</v>
+        <v>184</v>
       </c>
       <c r="C165" s="1" t="s">
-        <v>266</v>
+        <v>230</v>
       </c>
       <c r="D165" s="1">
         <v>1</v>
@@ -4131,10 +4148,13 @@
     </row>
     <row r="166" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A166" s="1" t="s">
-        <v>291</v>
+        <v>142</v>
       </c>
       <c r="B166" s="1" t="s">
-        <v>292</v>
+        <v>143</v>
+      </c>
+      <c r="C166" s="1" t="s">
+        <v>230</v>
       </c>
       <c r="D166" s="1">
         <v>1</v>
@@ -4142,13 +4162,10 @@
     </row>
     <row r="167" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A167" s="1" t="s">
-        <v>65</v>
+        <v>256</v>
       </c>
       <c r="B167" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="C167" s="1" t="s">
-        <v>324</v>
+        <v>257</v>
       </c>
       <c r="D167" s="1">
         <v>1</v>
@@ -4156,10 +4173,10 @@
     </row>
     <row r="168" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A168" s="1" t="s">
-        <v>112</v>
+        <v>20</v>
       </c>
       <c r="B168" s="1" t="s">
-        <v>113</v>
+        <v>21</v>
       </c>
       <c r="C168" s="1" t="s">
         <v>324</v>
@@ -4170,13 +4187,13 @@
     </row>
     <row r="169" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A169" s="1" t="s">
-        <v>110</v>
+        <v>315</v>
       </c>
       <c r="B169" s="1" t="s">
-        <v>111</v>
+        <v>316</v>
       </c>
       <c r="C169" s="1" t="s">
-        <v>324</v>
+        <v>317</v>
       </c>
       <c r="D169" s="1">
         <v>1</v>
@@ -4184,13 +4201,13 @@
     </row>
     <row r="170" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A170" s="1" t="s">
-        <v>233</v>
+        <v>189</v>
       </c>
       <c r="B170" s="1" t="s">
-        <v>234</v>
+        <v>190</v>
       </c>
       <c r="C170" s="1" t="s">
-        <v>326</v>
+        <v>230</v>
       </c>
       <c r="D170" s="1">
         <v>1</v>
@@ -4198,10 +4215,10 @@
     </row>
     <row r="171" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A171" s="1" t="s">
-        <v>202</v>
+        <v>162</v>
       </c>
       <c r="B171" s="1" t="s">
-        <v>203</v>
+        <v>161</v>
       </c>
       <c r="C171" s="1" t="s">
         <v>230</v>
@@ -4212,13 +4229,13 @@
     </row>
     <row r="172" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A172" s="1" t="s">
-        <v>26</v>
+        <v>241</v>
       </c>
       <c r="B172" s="1" t="s">
-        <v>27</v>
+        <v>242</v>
       </c>
       <c r="C172" s="1" t="s">
-        <v>324</v>
+        <v>326</v>
       </c>
       <c r="D172" s="1">
         <v>1</v>
@@ -4226,13 +4243,13 @@
     </row>
     <row r="173" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A173" s="1" t="s">
-        <v>28</v>
+        <v>452</v>
       </c>
       <c r="B173" s="1" t="s">
-        <v>29</v>
+        <v>453</v>
       </c>
       <c r="C173" s="1" t="s">
-        <v>324</v>
+        <v>415</v>
       </c>
       <c r="D173" s="1">
         <v>1</v>
@@ -4240,10 +4257,13 @@
     </row>
     <row r="174" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A174" s="1" t="s">
-        <v>287</v>
+        <v>71</v>
       </c>
       <c r="B174" s="1" t="s">
-        <v>288</v>
+        <v>72</v>
+      </c>
+      <c r="C174" s="1" t="s">
+        <v>324</v>
       </c>
       <c r="D174" s="1">
         <v>1</v>
@@ -4251,10 +4271,13 @@
     </row>
     <row r="175" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A175" s="1" t="s">
-        <v>283</v>
+        <v>144</v>
       </c>
       <c r="B175" s="1" t="s">
-        <v>284</v>
+        <v>145</v>
+      </c>
+      <c r="C175" s="1" t="s">
+        <v>230</v>
       </c>
       <c r="D175" s="1">
         <v>1</v>
@@ -4262,13 +4285,13 @@
     </row>
     <row r="176" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A176" s="1" t="s">
-        <v>63</v>
+        <v>213</v>
       </c>
       <c r="B176" s="1" t="s">
-        <v>64</v>
+        <v>214</v>
       </c>
       <c r="C176" s="1" t="s">
-        <v>324</v>
+        <v>230</v>
       </c>
       <c r="D176" s="1">
         <v>1</v>
@@ -4276,13 +4299,10 @@
     </row>
     <row r="177" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A177" s="1" t="s">
-        <v>330</v>
+        <v>278</v>
       </c>
       <c r="B177" s="1" t="s">
-        <v>331</v>
-      </c>
-      <c r="C177" s="1" t="s">
-        <v>249</v>
+        <v>279</v>
       </c>
       <c r="D177" s="1">
         <v>1</v>
@@ -4290,13 +4310,13 @@
     </row>
     <row r="178" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A178" s="1" t="s">
-        <v>362</v>
+        <v>348</v>
       </c>
       <c r="B178" s="1" t="s">
-        <v>361</v>
+        <v>349</v>
       </c>
       <c r="C178" s="1" t="s">
-        <v>266</v>
+        <v>340</v>
       </c>
       <c r="D178" s="1">
         <v>1</v>
@@ -4304,13 +4324,13 @@
     </row>
     <row r="179" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A179" s="1" t="s">
-        <v>362</v>
+        <v>226</v>
       </c>
       <c r="B179" s="1" t="s">
-        <v>363</v>
+        <v>227</v>
       </c>
       <c r="C179" s="1" t="s">
-        <v>341</v>
+        <v>230</v>
       </c>
       <c r="D179" s="1">
         <v>1</v>
@@ -4318,13 +4338,13 @@
     </row>
     <row r="180" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A180" s="1" t="s">
-        <v>364</v>
+        <v>6</v>
       </c>
       <c r="B180" s="1" t="s">
-        <v>365</v>
+        <v>7</v>
       </c>
       <c r="C180" s="1" t="s">
-        <v>266</v>
+        <v>326</v>
       </c>
       <c r="D180" s="1">
         <v>1</v>
@@ -4332,13 +4352,10 @@
     </row>
     <row r="181" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A181" s="1" t="s">
-        <v>366</v>
+        <v>299</v>
       </c>
       <c r="B181" s="1" t="s">
-        <v>367</v>
-      </c>
-      <c r="C181" s="1" t="s">
-        <v>266</v>
+        <v>300</v>
       </c>
       <c r="D181" s="1">
         <v>1</v>
@@ -4346,13 +4363,10 @@
     </row>
     <row r="182" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A182" s="1" t="s">
-        <v>368</v>
+        <v>305</v>
       </c>
       <c r="B182" s="1" t="s">
-        <v>369</v>
-      </c>
-      <c r="C182" s="1" t="s">
-        <v>356</v>
+        <v>306</v>
       </c>
       <c r="D182" s="1">
         <v>1</v>
@@ -4360,13 +4374,13 @@
     </row>
     <row r="183" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A183" s="1" t="s">
-        <v>370</v>
+        <v>388</v>
       </c>
       <c r="B183" s="1" t="s">
-        <v>371</v>
+        <v>389</v>
       </c>
       <c r="C183" s="1" t="s">
-        <v>372</v>
+        <v>415</v>
       </c>
       <c r="D183" s="1">
         <v>1</v>
@@ -4374,13 +4388,13 @@
     </row>
     <row r="184" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A184" s="1" t="s">
-        <v>373</v>
+        <v>403</v>
       </c>
       <c r="B184" s="1" t="s">
-        <v>374</v>
+        <v>404</v>
       </c>
       <c r="C184" s="1" t="s">
-        <v>356</v>
+        <v>415</v>
       </c>
       <c r="D184" s="1">
         <v>1</v>
@@ -4388,13 +4402,13 @@
     </row>
     <row r="185" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A185" s="1" t="s">
+        <v>374</v>
+      </c>
+      <c r="B185" s="1" t="s">
         <v>375</v>
       </c>
-      <c r="B185" s="1" t="s">
-        <v>376</v>
-      </c>
       <c r="C185" s="1" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="D185" s="1">
         <v>1</v>
@@ -4402,13 +4416,13 @@
     </row>
     <row r="186" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A186" s="1" t="s">
-        <v>379</v>
+        <v>102</v>
       </c>
       <c r="B186" s="1" t="s">
-        <v>380</v>
+        <v>103</v>
       </c>
       <c r="C186" s="1" t="s">
-        <v>230</v>
+        <v>324</v>
       </c>
       <c r="D186" s="1">
         <v>1</v>
@@ -4416,13 +4430,13 @@
     </row>
     <row r="187" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A187" s="1" t="s">
-        <v>382</v>
+        <v>104</v>
       </c>
       <c r="B187" s="1" t="s">
-        <v>381</v>
+        <v>105</v>
       </c>
       <c r="C187" s="1" t="s">
-        <v>230</v>
+        <v>324</v>
       </c>
       <c r="D187" s="1">
         <v>1</v>
@@ -4430,10 +4444,10 @@
     </row>
     <row r="188" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A188" s="1" t="s">
-        <v>383</v>
+        <v>228</v>
       </c>
       <c r="B188" s="1" t="s">
-        <v>384</v>
+        <v>229</v>
       </c>
       <c r="C188" s="1" t="s">
         <v>230</v>
@@ -4444,13 +4458,13 @@
     </row>
     <row r="189" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A189" s="1" t="s">
-        <v>385</v>
+        <v>52</v>
       </c>
       <c r="B189" s="1" t="s">
-        <v>386</v>
+        <v>53</v>
       </c>
       <c r="C189" s="1" t="s">
-        <v>230</v>
+        <v>324</v>
       </c>
       <c r="D189" s="1">
         <v>1</v>
@@ -4458,13 +4472,13 @@
     </row>
     <row r="190" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A190" s="1" t="s">
-        <v>387</v>
+        <v>50</v>
       </c>
       <c r="B190" s="1" t="s">
-        <v>388</v>
+        <v>51</v>
       </c>
       <c r="C190" s="1" t="s">
-        <v>417</v>
+        <v>324</v>
       </c>
       <c r="D190" s="1">
         <v>1</v>
@@ -4472,13 +4486,13 @@
     </row>
     <row r="191" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A191" s="1" t="s">
-        <v>389</v>
+        <v>150</v>
       </c>
       <c r="B191" s="1" t="s">
-        <v>390</v>
+        <v>151</v>
       </c>
       <c r="C191" s="1" t="s">
-        <v>417</v>
+        <v>230</v>
       </c>
       <c r="D191" s="1">
         <v>1</v>
@@ -4486,13 +4500,13 @@
     </row>
     <row r="192" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A192" s="1" t="s">
-        <v>391</v>
+        <v>204</v>
       </c>
       <c r="B192" s="1" t="s">
-        <v>392</v>
+        <v>205</v>
       </c>
       <c r="C192" s="1" t="s">
-        <v>356</v>
+        <v>230</v>
       </c>
       <c r="D192" s="1">
         <v>1</v>
@@ -4500,13 +4514,13 @@
     </row>
     <row r="193" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A193" s="1" t="s">
-        <v>393</v>
+        <v>169</v>
       </c>
       <c r="B193" s="1" t="s">
-        <v>394</v>
+        <v>170</v>
       </c>
       <c r="C193" s="1" t="s">
-        <v>356</v>
+        <v>230</v>
       </c>
       <c r="D193" s="1">
         <v>1</v>
@@ -4514,13 +4528,13 @@
     </row>
     <row r="194" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A194" s="1" t="s">
-        <v>395</v>
+        <v>152</v>
       </c>
       <c r="B194" s="1" t="s">
-        <v>396</v>
+        <v>153</v>
       </c>
       <c r="C194" s="1" t="s">
-        <v>356</v>
+        <v>230</v>
       </c>
       <c r="D194" s="1">
         <v>1</v>
@@ -4528,13 +4542,13 @@
     </row>
     <row r="195" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A195" s="1" t="s">
-        <v>397</v>
+        <v>171</v>
       </c>
       <c r="B195" s="1" t="s">
-        <v>398</v>
+        <v>172</v>
       </c>
       <c r="C195" s="1" t="s">
-        <v>356</v>
+        <v>230</v>
       </c>
       <c r="D195" s="1">
         <v>1</v>
@@ -4542,13 +4556,13 @@
     </row>
     <row r="196" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A196" s="1" t="s">
-        <v>399</v>
+        <v>134</v>
       </c>
       <c r="B196" s="1" t="s">
-        <v>400</v>
+        <v>135</v>
       </c>
       <c r="C196" s="1" t="s">
-        <v>401</v>
+        <v>230</v>
       </c>
       <c r="D196" s="1">
         <v>1</v>
@@ -4556,13 +4570,10 @@
     </row>
     <row r="197" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A197" s="1" t="s">
-        <v>402</v>
+        <v>272</v>
       </c>
       <c r="B197" s="1" t="s">
-        <v>403</v>
-      </c>
-      <c r="C197" s="1" t="s">
-        <v>356</v>
+        <v>275</v>
       </c>
       <c r="D197" s="1">
         <v>1</v>
@@ -4570,13 +4581,10 @@
     </row>
     <row r="198" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A198" s="1" t="s">
-        <v>404</v>
+        <v>265</v>
       </c>
       <c r="B198" s="1" t="s">
-        <v>405</v>
-      </c>
-      <c r="C198" s="1" t="s">
-        <v>417</v>
+        <v>265</v>
       </c>
       <c r="D198" s="1">
         <v>1</v>
@@ -4584,13 +4592,13 @@
     </row>
     <row r="199" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A199" s="1" t="s">
-        <v>406</v>
+        <v>136</v>
       </c>
       <c r="B199" s="1" t="s">
-        <v>407</v>
+        <v>137</v>
       </c>
       <c r="C199" s="1" t="s">
-        <v>401</v>
+        <v>230</v>
       </c>
       <c r="D199" s="1">
         <v>1</v>
@@ -4598,13 +4606,13 @@
     </row>
     <row r="200" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A200" s="1" t="s">
-        <v>408</v>
+        <v>138</v>
       </c>
       <c r="B200" s="1" t="s">
-        <v>409</v>
+        <v>139</v>
       </c>
       <c r="C200" s="1" t="s">
-        <v>410</v>
+        <v>230</v>
       </c>
       <c r="D200" s="1">
         <v>1</v>
@@ -4612,13 +4620,13 @@
     </row>
     <row r="201" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A201" s="1" t="s">
-        <v>267</v>
+        <v>140</v>
       </c>
       <c r="B201" s="1" t="s">
-        <v>411</v>
+        <v>141</v>
       </c>
       <c r="C201" s="1" t="s">
-        <v>412</v>
+        <v>230</v>
       </c>
       <c r="D201" s="1">
         <v>1</v>
@@ -4626,13 +4634,13 @@
     </row>
     <row r="202" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A202" s="1" t="s">
-        <v>413</v>
+        <v>361</v>
       </c>
       <c r="B202" s="1" t="s">
-        <v>414</v>
+        <v>360</v>
       </c>
       <c r="C202" s="1" t="s">
-        <v>401</v>
+        <v>266</v>
       </c>
       <c r="D202" s="1">
         <v>1</v>
@@ -4640,13 +4648,13 @@
     </row>
     <row r="203" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A203" s="1" t="s">
-        <v>415</v>
+        <v>361</v>
       </c>
       <c r="B203" s="1" t="s">
-        <v>416</v>
+        <v>362</v>
       </c>
       <c r="C203" s="1" t="s">
-        <v>378</v>
+        <v>340</v>
       </c>
       <c r="D203" s="1">
         <v>1</v>
@@ -4654,13 +4662,13 @@
     </row>
     <row r="204" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A204" s="1" t="s">
-        <v>418</v>
+        <v>129</v>
       </c>
       <c r="B204" s="1" t="s">
-        <v>419</v>
+        <v>130</v>
       </c>
       <c r="C204" s="1" t="s">
-        <v>377</v>
+        <v>230</v>
       </c>
       <c r="D204" s="1">
         <v>1</v>
@@ -4668,13 +4676,13 @@
     </row>
     <row r="205" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A205" s="1" t="s">
-        <v>420</v>
+        <v>318</v>
       </c>
       <c r="B205" s="1" t="s">
-        <v>421</v>
+        <v>319</v>
       </c>
       <c r="C205" s="1" t="s">
-        <v>410</v>
+        <v>249</v>
       </c>
       <c r="D205" s="1">
         <v>1</v>
@@ -4682,13 +4690,13 @@
     </row>
     <row r="206" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A206" s="1" t="s">
-        <v>422</v>
+        <v>59</v>
       </c>
       <c r="B206" s="1" t="s">
-        <v>423</v>
+        <v>60</v>
       </c>
       <c r="C206" s="1" t="s">
-        <v>356</v>
+        <v>324</v>
       </c>
       <c r="D206" s="1">
         <v>1</v>
@@ -4696,13 +4704,13 @@
     </row>
     <row r="207" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A207" s="1" t="s">
-        <v>424</v>
+        <v>320</v>
       </c>
       <c r="B207" s="1" t="s">
-        <v>425</v>
+        <v>321</v>
       </c>
       <c r="C207" s="1" t="s">
-        <v>426</v>
+        <v>359</v>
       </c>
       <c r="D207" s="1">
         <v>1</v>
@@ -4710,13 +4718,13 @@
     </row>
     <row r="208" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A208" s="1" t="s">
-        <v>427</v>
+        <v>356</v>
       </c>
       <c r="B208" s="1" t="s">
-        <v>428</v>
+        <v>357</v>
       </c>
       <c r="C208" s="1" t="s">
-        <v>377</v>
+        <v>358</v>
       </c>
       <c r="D208" s="1">
         <v>1</v>
@@ -4724,13 +4732,13 @@
     </row>
     <row r="209" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A209" s="1" t="s">
-        <v>429</v>
+        <v>158</v>
       </c>
       <c r="B209" s="1" t="s">
-        <v>430</v>
+        <v>159</v>
       </c>
       <c r="C209" s="1" t="s">
-        <v>325</v>
+        <v>230</v>
       </c>
       <c r="D209" s="1">
         <v>1</v>
@@ -4738,13 +4746,10 @@
     </row>
     <row r="210" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A210" s="1" t="s">
-        <v>431</v>
+        <v>270</v>
       </c>
       <c r="B210" s="1" t="s">
-        <v>432</v>
-      </c>
-      <c r="C210" s="1" t="s">
-        <v>417</v>
+        <v>271</v>
       </c>
       <c r="D210" s="1">
         <v>1</v>
@@ -4752,13 +4757,13 @@
     </row>
     <row r="211" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A211" s="1" t="s">
-        <v>433</v>
+        <v>322</v>
       </c>
       <c r="B211" s="1" t="s">
-        <v>434</v>
+        <v>323</v>
       </c>
       <c r="C211" s="1" t="s">
-        <v>377</v>
+        <v>324</v>
       </c>
       <c r="D211" s="1">
         <v>1</v>
@@ -4766,13 +4771,13 @@
     </row>
     <row r="212" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A212" s="1" t="s">
-        <v>435</v>
+        <v>146</v>
       </c>
       <c r="B212" s="1" t="s">
-        <v>436</v>
+        <v>147</v>
       </c>
       <c r="C212" s="1" t="s">
-        <v>410</v>
+        <v>230</v>
       </c>
       <c r="D212" s="1">
         <v>1</v>
@@ -4780,13 +4785,13 @@
     </row>
     <row r="213" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A213" s="1" t="s">
-        <v>437</v>
+        <v>40</v>
       </c>
       <c r="B213" s="1" t="s">
-        <v>438</v>
+        <v>41</v>
       </c>
       <c r="C213" s="1" t="s">
-        <v>410</v>
+        <v>324</v>
       </c>
       <c r="D213" s="1">
         <v>1</v>
@@ -4794,13 +4799,10 @@
     </row>
     <row r="214" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A214" s="1" t="s">
-        <v>439</v>
+        <v>280</v>
       </c>
       <c r="B214" s="1" t="s">
-        <v>440</v>
-      </c>
-      <c r="C214" s="1" t="s">
-        <v>353</v>
+        <v>281</v>
       </c>
       <c r="D214" s="1">
         <v>1</v>
@@ -4808,13 +4810,13 @@
     </row>
     <row r="215" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A215" s="1" t="s">
-        <v>441</v>
+        <v>369</v>
       </c>
       <c r="B215" s="1" t="s">
-        <v>442</v>
+        <v>370</v>
       </c>
       <c r="C215" s="1" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="D215" s="1">
         <v>1</v>
@@ -4822,13 +4824,13 @@
     </row>
     <row r="216" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A216" s="1" t="s">
-        <v>443</v>
+        <v>346</v>
       </c>
       <c r="B216" s="1" t="s">
-        <v>444</v>
+        <v>347</v>
       </c>
       <c r="C216" s="1" t="s">
-        <v>356</v>
+        <v>266</v>
       </c>
       <c r="D216" s="1">
         <v>1</v>
@@ -4836,13 +4838,13 @@
     </row>
     <row r="217" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A217" s="1" t="s">
-        <v>445</v>
+        <v>418</v>
       </c>
       <c r="B217" s="1" t="s">
-        <v>446</v>
+        <v>419</v>
       </c>
       <c r="C217" s="1" t="s">
-        <v>266</v>
+        <v>409</v>
       </c>
       <c r="D217" s="1">
         <v>1</v>
@@ -4850,13 +4852,13 @@
     </row>
     <row r="218" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A218" s="1" t="s">
-        <v>447</v>
+        <v>420</v>
       </c>
       <c r="B218" s="1" t="s">
-        <v>448</v>
+        <v>421</v>
       </c>
       <c r="C218" s="1" t="s">
-        <v>401</v>
+        <v>355</v>
       </c>
       <c r="D218" s="1">
         <v>1</v>
@@ -4864,13 +4866,10 @@
     </row>
     <row r="219" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A219" s="1" t="s">
-        <v>332</v>
+        <v>291</v>
       </c>
       <c r="B219" s="1" t="s">
-        <v>449</v>
-      </c>
-      <c r="C219" s="1" t="s">
-        <v>353</v>
+        <v>292</v>
       </c>
       <c r="D219" s="1">
         <v>1</v>
@@ -4878,13 +4877,13 @@
     </row>
     <row r="220" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A220" s="1" t="s">
-        <v>450</v>
+        <v>465</v>
       </c>
       <c r="B220" s="1" t="s">
-        <v>452</v>
+        <v>466</v>
       </c>
       <c r="C220" s="1" t="s">
-        <v>266</v>
+        <v>337</v>
       </c>
       <c r="D220" s="1">
         <v>1</v>
@@ -4892,13 +4891,13 @@
     </row>
     <row r="221" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A221" s="1" t="s">
-        <v>453</v>
+        <v>65</v>
       </c>
       <c r="B221" s="1" t="s">
-        <v>451</v>
+        <v>66</v>
       </c>
       <c r="C221" s="1" t="s">
-        <v>356</v>
+        <v>324</v>
       </c>
       <c r="D221" s="1">
         <v>1</v>
@@ -4906,13 +4905,13 @@
     </row>
     <row r="222" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A222" s="1" t="s">
-        <v>454</v>
+        <v>112</v>
       </c>
       <c r="B222" s="1" t="s">
-        <v>455</v>
+        <v>113</v>
       </c>
       <c r="C222" s="1" t="s">
-        <v>417</v>
+        <v>324</v>
       </c>
       <c r="D222" s="1">
         <v>1</v>
@@ -4920,13 +4919,13 @@
     </row>
     <row r="223" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A223" s="1" t="s">
-        <v>456</v>
+        <v>110</v>
       </c>
       <c r="B223" s="1" t="s">
-        <v>457</v>
+        <v>111</v>
       </c>
       <c r="C223" s="1" t="s">
-        <v>266</v>
+        <v>324</v>
       </c>
       <c r="D223" s="1">
         <v>1</v>
@@ -4934,13 +4933,13 @@
     </row>
     <row r="224" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A224" s="1" t="s">
-        <v>458</v>
+        <v>233</v>
       </c>
       <c r="B224" s="1" t="s">
-        <v>459</v>
+        <v>234</v>
       </c>
       <c r="C224" s="1" t="s">
-        <v>356</v>
+        <v>326</v>
       </c>
       <c r="D224" s="1">
         <v>1</v>
@@ -4948,13 +4947,13 @@
     </row>
     <row r="225" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A225" s="1" t="s">
-        <v>460</v>
+        <v>202</v>
       </c>
       <c r="B225" s="1" t="s">
-        <v>459</v>
+        <v>203</v>
       </c>
       <c r="C225" s="1" t="s">
-        <v>356</v>
+        <v>230</v>
       </c>
       <c r="D225" s="1">
         <v>1</v>
@@ -4962,13 +4961,13 @@
     </row>
     <row r="226" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A226" s="1" t="s">
-        <v>461</v>
+        <v>26</v>
       </c>
       <c r="B226" s="1" t="s">
-        <v>462</v>
+        <v>27</v>
       </c>
       <c r="C226" s="1" t="s">
-        <v>266</v>
+        <v>324</v>
       </c>
       <c r="D226" s="1">
         <v>1</v>
@@ -4976,13 +4975,13 @@
     </row>
     <row r="227" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A227" s="1" t="s">
-        <v>463</v>
+        <v>28</v>
       </c>
       <c r="B227" s="1" t="s">
-        <v>464</v>
+        <v>29</v>
       </c>
       <c r="C227" s="1" t="s">
-        <v>266</v>
+        <v>324</v>
       </c>
       <c r="D227" s="1">
         <v>1</v>
@@ -4990,13 +4989,10 @@
     </row>
     <row r="228" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A228" s="1" t="s">
-        <v>465</v>
+        <v>287</v>
       </c>
       <c r="B228" s="1" t="s">
-        <v>466</v>
-      </c>
-      <c r="C228" s="1" t="s">
-        <v>266</v>
+        <v>288</v>
       </c>
       <c r="D228" s="1">
         <v>1</v>
@@ -5004,13 +5000,10 @@
     </row>
     <row r="229" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A229" s="1" t="s">
-        <v>467</v>
+        <v>283</v>
       </c>
       <c r="B229" s="1" t="s">
-        <v>468</v>
-      </c>
-      <c r="C229" s="1" t="s">
-        <v>338</v>
+        <v>284</v>
       </c>
       <c r="D229" s="1">
         <v>1</v>
@@ -5018,13 +5011,13 @@
     </row>
     <row r="230" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A230" s="1" t="s">
-        <v>469</v>
+        <v>461</v>
       </c>
       <c r="B230" s="1" t="s">
-        <v>470</v>
+        <v>462</v>
       </c>
       <c r="C230" s="1" t="s">
-        <v>353</v>
+        <v>266</v>
       </c>
       <c r="D230" s="1">
         <v>1</v>
@@ -5032,13 +5025,13 @@
     </row>
     <row r="231" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A231" s="1" t="s">
-        <v>471</v>
+        <v>63</v>
       </c>
       <c r="B231" s="1" t="s">
-        <v>472</v>
+        <v>64</v>
       </c>
       <c r="C231" s="1" t="s">
-        <v>359</v>
+        <v>324</v>
       </c>
       <c r="D231" s="1">
         <v>1</v>
@@ -5046,29 +5039,15 @@
     </row>
     <row r="232" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A232" s="1" t="s">
-        <v>473</v>
+        <v>330</v>
       </c>
       <c r="B232" s="1" t="s">
-        <v>474</v>
+        <v>331</v>
       </c>
       <c r="C232" s="1" t="s">
-        <v>356</v>
+        <v>249</v>
       </c>
       <c r="D232" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="233" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A233" s="1" t="s">
-        <v>475</v>
-      </c>
-      <c r="B233" s="1" t="s">
-        <v>476</v>
-      </c>
-      <c r="C233" s="1" t="s">
-        <v>477</v>
-      </c>
-      <c r="D233" s="1">
         <v>1</v>
       </c>
     </row>

</xml_diff>